<commit_message>
Fixed some files for February
</commit_message>
<xml_diff>
--- a/data/xlsx/02012019.xlsx
+++ b/data/xlsx/02012019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\tiffany\susa\web-dev\police-logs\cleaned\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AD3BBACA-44D3-48DB-A0F3-901FDC17DB3A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{64A3924A-1595-4C1F-9721-7A1C412137E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" xr2:uid="{3F3E0E46-A0AD-4629-ADAE-21D9BD89B34F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6825" xr2:uid="{05FF5AA9-5C4D-4379-A8F5-11775D51F4FA}"/>
   </bookViews>
   <sheets>
     <sheet name="02012019" sheetId="1" r:id="rId1"/>
@@ -394,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -408,6 +408,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -729,11 +730,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12531706-FD44-4B95-B3AC-B343B748C3AE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FE4B87A-9425-4F4D-BD64-1219AAD29392}">
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,11 +943,11 @@
       <c r="E8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="8">
-        <v>0</v>
-      </c>
-      <c r="G8" s="8">
-        <v>0</v>
+      <c r="F8" s="9">
+        <v>37.873187999999999</v>
+      </c>
+      <c r="G8" s="9">
+        <v>-122.30207299999999</v>
       </c>
       <c r="H8" s="5" t="s">
         <v>32</v>
@@ -972,7 +973,7 @@
       <c r="F9" s="6">
         <v>37.869556000000003</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="10">
         <v>-122.259337</v>
       </c>
       <c r="H9" s="5" t="s">
@@ -999,7 +1000,7 @@
       <c r="F10" s="6">
         <v>37.868706000000003</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="10">
         <v>-122.259184</v>
       </c>
       <c r="H10" s="7" t="s">
@@ -1088,7 +1089,7 @@
       </c>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>43497</v>
       </c>
@@ -1104,18 +1105,18 @@
       <c r="E14" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="8">
-        <v>0</v>
-      </c>
-      <c r="G14" s="8">
-        <v>0</v>
+      <c r="F14" s="6">
+        <v>37.867052999999999</v>
+      </c>
+      <c r="G14" s="6">
+        <v>-122.25618299999999</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>51</v>
       </c>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>43497</v>
       </c>
@@ -1131,11 +1132,11 @@
       <c r="E15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="8">
-        <v>0</v>
-      </c>
-      <c r="G15" s="8">
-        <v>0</v>
+      <c r="F15" s="9">
+        <v>37.866230000000002</v>
+      </c>
+      <c r="G15" s="9">
+        <v>-122.25484400000001</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>11</v>
@@ -1152,17 +1153,17 @@
       <c r="C16" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="11" t="s">
         <v>56</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="8">
-        <v>0</v>
-      </c>
-      <c r="G16" s="8">
-        <v>0</v>
+      <c r="F16" s="6">
+        <v>37.874133</v>
+      </c>
+      <c r="G16" s="6">
+        <v>-122.241964</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>11</v>
@@ -1371,16 +1372,16 @@
       <c r="A26" s="5"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="11"/>
+      <c r="A28" s="12"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="12"/>
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
+      <c r="A30" s="13"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+      <c r="G30" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>